<commit_message>
large rerun fixes #61
excluding 2021, time window of 5 years for exp, moving graphics to 16.Rmd
</commit_message>
<xml_diff>
--- a/paper/table1.xlsx
+++ b/paper/table1.xlsx
@@ -398,16 +398,16 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>75222</v>
+        <v>73077</v>
       </c>
       <c r="D2" t="n">
         <v>81824</v>
       </c>
       <c r="E2" t="n">
-        <v>6602</v>
+        <v>8747</v>
       </c>
       <c r="F2" t="n">
-        <v>8.8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -418,16 +418,16 @@
         <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>58341</v>
+        <v>58397</v>
       </c>
       <c r="D3" t="n">
         <v>61805</v>
       </c>
       <c r="E3" t="n">
-        <v>3464</v>
+        <v>3408</v>
       </c>
       <c r="F3" t="n">
-        <v>5.9</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="4">
@@ -438,16 +438,16 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>447871</v>
+        <v>451779</v>
       </c>
       <c r="D4" t="n">
         <v>695758</v>
       </c>
       <c r="E4" t="n">
-        <v>247887</v>
+        <v>243979</v>
       </c>
       <c r="F4" t="n">
-        <v>55.3</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
@@ -458,16 +458,16 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>78748</v>
+        <v>78642</v>
       </c>
       <c r="D5" t="n">
         <v>104591</v>
       </c>
       <c r="E5" t="n">
-        <v>25843</v>
+        <v>25949</v>
       </c>
       <c r="F5" t="n">
-        <v>32.8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
@@ -478,16 +478,16 @@
         <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>49837</v>
+        <v>50473</v>
       </c>
       <c r="D6" t="n">
         <v>75034</v>
       </c>
       <c r="E6" t="n">
-        <v>25197</v>
+        <v>24561</v>
       </c>
       <c r="F6" t="n">
-        <v>50.6</v>
+        <v>48.7</v>
       </c>
     </row>
     <row r="7">
@@ -498,16 +498,16 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>263572</v>
+        <v>282888</v>
       </c>
       <c r="D7" t="n">
         <v>293502</v>
       </c>
       <c r="E7" t="n">
-        <v>29930</v>
+        <v>10614</v>
       </c>
       <c r="F7" t="n">
-        <v>11.4</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="8">
@@ -518,16 +518,16 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>68486</v>
+        <v>70064</v>
       </c>
       <c r="D8" t="n">
         <v>73132</v>
       </c>
       <c r="E8" t="n">
-        <v>4646</v>
+        <v>3068</v>
       </c>
       <c r="F8" t="n">
-        <v>6.8</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="9">
@@ -538,16 +538,16 @@
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>49950</v>
+        <v>52280</v>
       </c>
       <c r="D9" t="n">
         <v>51066</v>
       </c>
       <c r="E9" t="n">
-        <v>1116</v>
+        <v>-1214</v>
       </c>
       <c r="F9" t="n">
-        <v>2.2</v>
+        <v>-2.3</v>
       </c>
     </row>
     <row r="10">
@@ -558,16 +558,16 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>439374</v>
+        <v>425484</v>
       </c>
       <c r="D10" t="n">
-        <v>479760</v>
+        <v>494604</v>
       </c>
       <c r="E10" t="n">
-        <v>40386</v>
+        <v>69120</v>
       </c>
       <c r="F10" t="n">
-        <v>9.2</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="11">
@@ -578,16 +578,16 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>90086</v>
+        <v>88975</v>
       </c>
       <c r="D11" t="n">
-        <v>97870</v>
+        <v>95411</v>
       </c>
       <c r="E11" t="n">
-        <v>7784</v>
+        <v>6436</v>
       </c>
       <c r="F11" t="n">
-        <v>8.6</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="12">
@@ -598,16 +598,16 @@
         <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>68498</v>
+        <v>67893</v>
       </c>
       <c r="D12" t="n">
-        <v>75570</v>
+        <v>75971</v>
       </c>
       <c r="E12" t="n">
-        <v>7072</v>
+        <v>8078</v>
       </c>
       <c r="F12" t="n">
-        <v>10.3</v>
+        <v>11.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data and name updates
</commit_message>
<xml_diff>
--- a/paper/table1.xlsx
+++ b/paper/table1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -363,10 +363,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -561,13 +561,13 @@
         <v>425484</v>
       </c>
       <c r="D10" t="n">
-        <v>494604</v>
+        <v>479760</v>
       </c>
       <c r="E10" t="n">
-        <v>69120</v>
+        <v>54276</v>
       </c>
       <c r="F10" t="n">
-        <v>16.2</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="11">
@@ -581,13 +581,13 @@
         <v>88975</v>
       </c>
       <c r="D11" t="n">
-        <v>95411</v>
+        <v>97870</v>
       </c>
       <c r="E11" t="n">
-        <v>6436</v>
+        <v>8895</v>
       </c>
       <c r="F11" t="n">
-        <v>7.2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -598,16 +598,16 @@
         <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>67893</v>
+        <v>67445</v>
       </c>
       <c r="D12" t="n">
-        <v>75971</v>
+        <v>75570</v>
       </c>
       <c r="E12" t="n">
-        <v>8078</v>
+        <v>8125</v>
       </c>
       <c r="F12" t="n">
-        <v>11.9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>